<commit_message>
Randomized the record order
Randomized the record order to make it work on the decision tree analysis.
</commit_message>
<xml_diff>
--- a/docs/analysis/data/Iris.xlsx
+++ b/docs/analysis/data/Iris.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amo.QTSEL\Documents\Qlik\Sense\Extensions\advanced-analytics-toolbox\docs\analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Masaki Hamano\Documents\Qlik\Sense\Extensions\advanced-analytics-toolbox\docs\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -442,7 +442,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -480,13 +480,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5.0999999999999996</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="D2">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="E2">
         <v>0.2</v>
@@ -500,19 +500,19 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>3.8</v>
       </c>
       <c r="D3">
-        <v>1.4</v>
+        <v>6.4</v>
       </c>
       <c r="E3">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -520,19 +520,19 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4.7</v>
+        <v>6.2</v>
       </c>
       <c r="C4">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="D4">
-        <v>1.3</v>
+        <v>5.4</v>
       </c>
       <c r="E4">
-        <v>0.2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
@@ -540,19 +540,19 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4.5999999999999996</v>
+        <v>6.7</v>
       </c>
       <c r="C5">
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
       <c r="D5">
-        <v>1.5</v>
+        <v>5.8</v>
       </c>
       <c r="E5">
-        <v>0.2</v>
+        <v>1.8</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -560,19 +560,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>5.7</v>
       </c>
       <c r="C6">
-        <v>3.6</v>
+        <v>2.8</v>
       </c>
       <c r="D6">
-        <v>1.4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E6">
-        <v>0.2</v>
+        <v>1.3</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -580,16 +580,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>5.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C7">
-        <v>3.9</v>
+        <v>3.3</v>
       </c>
       <c r="D7">
         <v>1.7</v>
       </c>
       <c r="E7">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
@@ -600,19 +600,19 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4.5999999999999996</v>
+        <v>6.2</v>
       </c>
       <c r="C8">
-        <v>3.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D8">
-        <v>1.4</v>
+        <v>4.5</v>
       </c>
       <c r="E8">
-        <v>0.3</v>
+        <v>1.5</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -620,19 +620,19 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>5.7</v>
       </c>
       <c r="C9">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>1.5</v>
+        <v>4.2</v>
       </c>
       <c r="E9">
-        <v>0.2</v>
+        <v>1.2</v>
       </c>
       <c r="F9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
@@ -640,19 +640,19 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>4.4000000000000004</v>
+        <v>7.2</v>
       </c>
       <c r="C10">
-        <v>2.9</v>
+        <v>3.6</v>
       </c>
       <c r="D10">
-        <v>1.4</v>
+        <v>6.1</v>
       </c>
       <c r="E10">
-        <v>0.2</v>
+        <v>2.5</v>
       </c>
       <c r="F10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -660,19 +660,19 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4.9000000000000004</v>
+        <v>7.4</v>
       </c>
       <c r="C11">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="D11">
-        <v>1.5</v>
+        <v>6.1</v>
       </c>
       <c r="E11">
-        <v>0.1</v>
+        <v>1.9</v>
       </c>
       <c r="F11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
@@ -680,19 +680,19 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>5.4</v>
+        <v>6.4</v>
       </c>
       <c r="C12">
-        <v>3.7</v>
+        <v>3.2</v>
       </c>
       <c r="D12">
-        <v>1.5</v>
+        <v>5.3</v>
       </c>
       <c r="E12">
-        <v>0.2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
@@ -700,16 +700,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>4.8</v>
+        <v>4.3</v>
       </c>
       <c r="C13">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>1.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E13">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
@@ -720,19 +720,19 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="D14">
-        <v>1.4</v>
+        <v>3.7</v>
       </c>
       <c r="E14">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
@@ -740,19 +740,19 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>4.3</v>
+        <v>6.3</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="D15">
-        <v>1.1000000000000001</v>
+        <v>4.7</v>
       </c>
       <c r="E15">
-        <v>0.1</v>
+        <v>1.6</v>
       </c>
       <c r="F15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
@@ -760,19 +760,19 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>5.8</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>1.2</v>
+        <v>3.5</v>
       </c>
       <c r="E16">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
@@ -780,10 +780,10 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>5.7</v>
+        <v>5.4</v>
       </c>
       <c r="C17">
-        <v>4.4000000000000004</v>
+        <v>3.4</v>
       </c>
       <c r="D17">
         <v>1.5</v>
@@ -800,19 +800,19 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>5.4</v>
+        <v>6.5</v>
       </c>
       <c r="C18">
-        <v>3.9</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>1.3</v>
+        <v>5.5</v>
       </c>
       <c r="E18">
-        <v>0.4</v>
+        <v>1.8</v>
       </c>
       <c r="F18" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
@@ -820,19 +820,19 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>5.0999999999999996</v>
+        <v>6.9</v>
       </c>
       <c r="C19">
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="D19">
-        <v>1.4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E19">
-        <v>0.3</v>
+        <v>1.5</v>
       </c>
       <c r="F19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
@@ -840,19 +840,19 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>5.7</v>
+        <v>5.5</v>
       </c>
       <c r="C20">
-        <v>3.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D20">
-        <v>1.7</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>0.3</v>
+        <v>1.3</v>
       </c>
       <c r="F20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
@@ -860,16 +860,16 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>5.0999999999999996</v>
+        <v>4.7</v>
       </c>
       <c r="C21">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
       <c r="D21">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="E21">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>
@@ -880,13 +880,13 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>5.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C22">
         <v>3.4</v>
       </c>
       <c r="D22">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="E22">
         <v>0.2</v>
@@ -900,19 +900,19 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>5.0999999999999996</v>
+        <v>6.8</v>
       </c>
       <c r="C23">
-        <v>3.7</v>
+        <v>2.8</v>
       </c>
       <c r="D23">
-        <v>1.5</v>
+        <v>4.8</v>
       </c>
       <c r="E23">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="F23" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
@@ -920,19 +920,19 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>4.5999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="C24">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>5.6</v>
       </c>
       <c r="E24">
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="F24" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
@@ -940,19 +940,19 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>5.0999999999999996</v>
+        <v>6.5</v>
       </c>
       <c r="C25">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>1.7</v>
+        <v>5.8</v>
       </c>
       <c r="E25">
-        <v>0.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F25" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
@@ -960,16 +960,16 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>4.8</v>
+        <v>5.4</v>
       </c>
       <c r="C26">
-        <v>3.4</v>
+        <v>3.9</v>
       </c>
       <c r="D26">
-        <v>1.9</v>
+        <v>1.3</v>
       </c>
       <c r="E26">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F26" t="s">
         <v>5</v>
@@ -980,13 +980,13 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D27">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="E27">
         <v>0.2</v>
@@ -1000,19 +1000,19 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>5.8</v>
       </c>
       <c r="C28">
-        <v>3.4</v>
+        <v>2.7</v>
       </c>
       <c r="D28">
-        <v>1.6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E28">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
@@ -1020,19 +1020,19 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>5.2</v>
+        <v>7.2</v>
       </c>
       <c r="C29">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="D29">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="E29">
-        <v>0.2</v>
+        <v>1.8</v>
       </c>
       <c r="F29" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
@@ -1060,16 +1060,16 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>4.7</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C31">
-        <v>3.2</v>
+        <v>3.7</v>
       </c>
       <c r="D31">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="E31">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F31" t="s">
         <v>5</v>
@@ -1080,16 +1080,16 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>4.8</v>
+        <v>5.7</v>
       </c>
       <c r="C32">
-        <v>3.1</v>
+        <v>3.8</v>
       </c>
       <c r="D32">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="E32">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F32" t="s">
         <v>5</v>
@@ -1100,19 +1100,19 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>5.4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C33">
-        <v>3.4</v>
+        <v>2.5</v>
       </c>
       <c r="D33">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="E33">
-        <v>0.4</v>
+        <v>1.7</v>
       </c>
       <c r="F33" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.4">
@@ -1120,19 +1120,19 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>5.2</v>
+        <v>6.3</v>
       </c>
       <c r="C34">
-        <v>4.0999999999999996</v>
+        <v>3.4</v>
       </c>
       <c r="D34">
-        <v>1.5</v>
+        <v>5.6</v>
       </c>
       <c r="E34">
-        <v>0.1</v>
+        <v>2.4</v>
       </c>
       <c r="F34" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.4">
@@ -1140,13 +1140,13 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>5.5</v>
+        <v>5.3</v>
       </c>
       <c r="C35">
-        <v>4.2</v>
+        <v>3.7</v>
       </c>
       <c r="D35">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="E35">
         <v>0.2</v>
@@ -1160,19 +1160,19 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>4.9000000000000004</v>
+        <v>7.2</v>
       </c>
       <c r="C36">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>1.5</v>
+        <v>5.8</v>
       </c>
       <c r="E36">
-        <v>0.2</v>
+        <v>1.6</v>
       </c>
       <c r="F36" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.4">
@@ -1180,19 +1180,19 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>6.3</v>
       </c>
       <c r="C37">
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
       <c r="D37">
-        <v>1.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E37">
-        <v>0.2</v>
+        <v>1.5</v>
       </c>
       <c r="F37" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.4">
@@ -1200,19 +1200,19 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="C38">
-        <v>3.5</v>
+        <v>2.9</v>
       </c>
       <c r="D38">
-        <v>1.3</v>
+        <v>4.7</v>
       </c>
       <c r="E38">
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="F38" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.4">
@@ -1220,19 +1220,19 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>4.9000000000000004</v>
+        <v>6.7</v>
       </c>
       <c r="C39">
-        <v>3.6</v>
+        <v>3</v>
       </c>
       <c r="D39">
-        <v>1.4</v>
+        <v>5</v>
       </c>
       <c r="E39">
-        <v>0.1</v>
+        <v>1.7</v>
       </c>
       <c r="F39" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.4">
@@ -1240,16 +1240,16 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>4.4000000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D40">
         <v>1.3</v>
       </c>
       <c r="E40">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F40" t="s">
         <v>5</v>
@@ -1260,19 +1260,19 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>5.0999999999999996</v>
+        <v>7</v>
       </c>
       <c r="C41">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="D41">
-        <v>1.5</v>
+        <v>4.7</v>
       </c>
       <c r="E41">
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="F41" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.4">
@@ -1280,19 +1280,19 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>7.1</v>
       </c>
       <c r="C42">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D42">
-        <v>1.3</v>
+        <v>5.9</v>
       </c>
       <c r="E42">
-        <v>0.3</v>
+        <v>2.1</v>
       </c>
       <c r="F42" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.4">
@@ -1300,19 +1300,19 @@
         <v>42</v>
       </c>
       <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43">
+        <v>3.4</v>
+      </c>
+      <c r="D43">
         <v>4.5</v>
       </c>
-      <c r="C43">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D43">
-        <v>1.3</v>
-      </c>
       <c r="E43">
-        <v>0.3</v>
+        <v>1.6</v>
       </c>
       <c r="F43" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.4">
@@ -1320,16 +1320,16 @@
         <v>43</v>
       </c>
       <c r="B44">
+        <v>5.7</v>
+      </c>
+      <c r="C44">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C44">
-        <v>3.2</v>
-      </c>
       <c r="D44">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E44">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F44" t="s">
         <v>5</v>
@@ -1343,13 +1343,13 @@
         <v>5</v>
       </c>
       <c r="C45">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D45">
         <v>1.6</v>
       </c>
       <c r="E45">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="F45" t="s">
         <v>5</v>
@@ -1360,19 +1360,19 @@
         <v>45</v>
       </c>
       <c r="B46">
+        <v>6.9</v>
+      </c>
+      <c r="C46">
+        <v>3.1</v>
+      </c>
+      <c r="D46">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C46">
-        <v>3.8</v>
-      </c>
-      <c r="D46">
-        <v>1.9</v>
-      </c>
       <c r="E46">
-        <v>0.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F46" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.4">
@@ -1380,16 +1380,16 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>4.8</v>
+        <v>5.2</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D47">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="E47">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="F47" t="s">
         <v>5</v>
@@ -1400,19 +1400,19 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>5.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C48">
-        <v>3.8</v>
+        <v>2.4</v>
       </c>
       <c r="D48">
-        <v>1.6</v>
+        <v>3.3</v>
       </c>
       <c r="E48">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.4">
@@ -1420,16 +1420,16 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>4.5999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C49">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="D49">
         <v>1.4</v>
       </c>
       <c r="E49">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F49" t="s">
         <v>5</v>
@@ -1440,13 +1440,13 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>5.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C50">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="D50">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="E50">
         <v>0.2</v>
@@ -1460,19 +1460,19 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>5</v>
+        <v>6.4</v>
       </c>
       <c r="C51">
-        <v>3.3</v>
+        <v>2.9</v>
       </c>
       <c r="D51">
-        <v>1.4</v>
+        <v>4.3</v>
       </c>
       <c r="E51">
-        <v>0.2</v>
+        <v>1.3</v>
       </c>
       <c r="F51" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.4">
@@ -1480,19 +1480,19 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>7</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C52">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="D52">
-        <v>4.7</v>
+        <v>1.4</v>
       </c>
       <c r="E52">
-        <v>1.4</v>
+        <v>0.2</v>
       </c>
       <c r="F52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.4">
@@ -1500,19 +1500,19 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>6.4</v>
+        <v>5</v>
       </c>
       <c r="C53">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="D53">
-        <v>4.5</v>
+        <v>1.4</v>
       </c>
       <c r="E53">
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
       <c r="F53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.4">
@@ -1520,16 +1520,16 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>6.9</v>
+        <v>5.8</v>
       </c>
       <c r="C54">
-        <v>3.1</v>
+        <v>2.7</v>
       </c>
       <c r="D54">
-        <v>4.9000000000000004</v>
+        <v>3.9</v>
       </c>
       <c r="E54">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="F54" t="s">
         <v>6</v>
@@ -1540,19 +1540,19 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="C55">
-        <v>2.2999999999999998</v>
+        <v>3</v>
       </c>
       <c r="D55">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="E55">
-        <v>1.3</v>
+        <v>1.8</v>
       </c>
       <c r="F55" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.4">
@@ -1560,19 +1560,19 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>6.5</v>
+        <v>6.8</v>
       </c>
       <c r="C56">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="D56">
-        <v>4.5999999999999996</v>
+        <v>5.9</v>
       </c>
       <c r="E56">
-        <v>1.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F56" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.4">
@@ -1580,19 +1580,19 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>5.7</v>
+        <v>6.4</v>
       </c>
       <c r="C57">
         <v>2.8</v>
       </c>
       <c r="D57">
-        <v>4.5</v>
+        <v>5.6</v>
       </c>
       <c r="E57">
-        <v>1.3</v>
+        <v>2.1</v>
       </c>
       <c r="F57" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.4">
@@ -1600,16 +1600,16 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>6.3</v>
+        <v>6.6</v>
       </c>
       <c r="C58">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="D58">
-        <v>4.7</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E58">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="F58" t="s">
         <v>6</v>
@@ -1620,16 +1620,16 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>4.9000000000000004</v>
+        <v>6</v>
       </c>
       <c r="C59">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
       <c r="D59">
-        <v>3.3</v>
+        <v>4.5</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F59" t="s">
         <v>6</v>
@@ -1640,19 +1640,19 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
       <c r="C60">
-        <v>2.9</v>
+        <v>3.3</v>
       </c>
       <c r="D60">
-        <v>4.5999999999999996</v>
+        <v>5.7</v>
       </c>
       <c r="E60">
-        <v>1.3</v>
+        <v>2.5</v>
       </c>
       <c r="F60" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.4">
@@ -1660,19 +1660,19 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>5.2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C61">
-        <v>2.7</v>
+        <v>3.4</v>
       </c>
       <c r="D61">
-        <v>3.9</v>
+        <v>1.4</v>
       </c>
       <c r="E61">
-        <v>1.4</v>
+        <v>0.3</v>
       </c>
       <c r="F61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.4">
@@ -1680,19 +1680,19 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="D62">
-        <v>3.5</v>
+        <v>1.9</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.4">
@@ -1700,19 +1700,19 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>5.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="D63">
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="E63">
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="F63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.4">
@@ -1720,19 +1720,19 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>6</v>
+        <v>4.8</v>
       </c>
       <c r="C64">
-        <v>2.2000000000000002</v>
+        <v>3</v>
       </c>
       <c r="D64">
-        <v>4</v>
+        <v>1.4</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.4">
@@ -1740,16 +1740,16 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>6.1</v>
+        <v>5.7</v>
       </c>
       <c r="C65">
         <v>2.9</v>
       </c>
       <c r="D65">
-        <v>4.7</v>
+        <v>4.2</v>
       </c>
       <c r="E65">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="F65" t="s">
         <v>6</v>
@@ -1780,16 +1780,16 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>6.7</v>
+        <v>5.6</v>
       </c>
       <c r="C67">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="D67">
-        <v>4.4000000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="E67">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="F67" t="s">
         <v>6</v>
@@ -1800,19 +1800,19 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>5.6</v>
+        <v>5</v>
       </c>
       <c r="C68">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="D68">
-        <v>4.5</v>
+        <v>1.4</v>
       </c>
       <c r="E68">
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
       <c r="F68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.4">
@@ -1820,16 +1820,16 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>5.8</v>
+        <v>6.1</v>
       </c>
       <c r="C69">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
       <c r="D69">
-        <v>4.0999999999999996</v>
+        <v>4</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="F69" t="s">
         <v>6</v>
@@ -1840,19 +1840,19 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>6.2</v>
+        <v>5.8</v>
       </c>
       <c r="C70">
-        <v>2.2000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="D70">
-        <v>4.5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E70">
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="F70" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.4">
@@ -1860,16 +1860,16 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
       <c r="C71">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="D71">
-        <v>3.9</v>
+        <v>4.5</v>
       </c>
       <c r="E71">
-        <v>1.1000000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="F71" t="s">
         <v>6</v>
@@ -1880,19 +1880,19 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>5.9</v>
+        <v>5.8</v>
       </c>
       <c r="C72">
-        <v>3.2</v>
+        <v>2.7</v>
       </c>
       <c r="D72">
-        <v>4.8</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E72">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="F72" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.4">
@@ -1900,19 +1900,19 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>6.1</v>
+        <v>5.4</v>
       </c>
       <c r="C73">
-        <v>2.8</v>
+        <v>3.9</v>
       </c>
       <c r="D73">
-        <v>4</v>
+        <v>1.7</v>
       </c>
       <c r="E73">
-        <v>1.3</v>
+        <v>0.4</v>
       </c>
       <c r="F73" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.4">
@@ -1920,19 +1920,19 @@
         <v>73</v>
       </c>
       <c r="B74">
+        <v>7.3</v>
+      </c>
+      <c r="C74">
+        <v>2.9</v>
+      </c>
+      <c r="D74">
         <v>6.3</v>
       </c>
-      <c r="C74">
-        <v>2.5</v>
-      </c>
-      <c r="D74">
-        <v>4.9000000000000004</v>
-      </c>
       <c r="E74">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="F74" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.4">
@@ -1940,19 +1940,19 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>6.1</v>
+        <v>5.5</v>
       </c>
       <c r="C75">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="D75">
-        <v>4.7</v>
+        <v>1.3</v>
       </c>
       <c r="E75">
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
       <c r="F75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.4">
@@ -1960,19 +1960,19 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>6.4</v>
+        <v>5.7</v>
       </c>
       <c r="C76">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="D76">
-        <v>4.3</v>
+        <v>5</v>
       </c>
       <c r="E76">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.4">
@@ -1980,19 +1980,19 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>6.6</v>
+        <v>6.4</v>
       </c>
       <c r="C77">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="D77">
-        <v>4.4000000000000004</v>
+        <v>5.6</v>
       </c>
       <c r="E77">
-        <v>1.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F77" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.4">
@@ -2000,19 +2000,19 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>6.8</v>
+        <v>6.1</v>
       </c>
       <c r="C78">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="D78">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E78">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="F78" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.4">
@@ -2023,13 +2023,13 @@
         <v>6.7</v>
       </c>
       <c r="C79">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="D79">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="E79">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="F79" t="s">
         <v>6</v>
@@ -2040,19 +2040,19 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="C80">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="D80">
-        <v>4.5</v>
+        <v>5.3</v>
       </c>
       <c r="E80">
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="F80" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.4">
@@ -2060,16 +2060,16 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>5.7</v>
+        <v>5.9</v>
       </c>
       <c r="C81">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="D81">
-        <v>3.5</v>
+        <v>4.8</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="F81" t="s">
         <v>6</v>
@@ -2080,19 +2080,19 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>5.5</v>
+        <v>4.8</v>
       </c>
       <c r="C82">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
       <c r="D82">
-        <v>3.8</v>
+        <v>1.6</v>
       </c>
       <c r="E82">
-        <v>1.1000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="F82" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.4">
@@ -2100,16 +2100,16 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>5.5</v>
+        <v>5.8</v>
       </c>
       <c r="C83">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="D83">
-        <v>3.7</v>
+        <v>4</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F83" t="s">
         <v>6</v>
@@ -2120,16 +2120,16 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>5.8</v>
+        <v>5.5</v>
       </c>
       <c r="C84">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="D84">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="E84">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="F84" t="s">
         <v>6</v>
@@ -2140,19 +2140,19 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>6</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C85">
-        <v>2.7</v>
+        <v>3.5</v>
       </c>
       <c r="D85">
-        <v>5.0999999999999996</v>
+        <v>1.4</v>
       </c>
       <c r="E85">
-        <v>1.6</v>
+        <v>0.3</v>
       </c>
       <c r="F85" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.4">
@@ -2160,16 +2160,16 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>5.4</v>
+        <v>5.5</v>
       </c>
       <c r="C86">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="D86">
-        <v>4.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E86">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="F86" t="s">
         <v>6</v>
@@ -2180,16 +2180,16 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>6</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C87">
-        <v>3.4</v>
+        <v>2.5</v>
       </c>
       <c r="D87">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="E87">
-        <v>1.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F87" t="s">
         <v>6</v>
@@ -2200,19 +2200,19 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>6.7</v>
+        <v>5.9</v>
       </c>
       <c r="C88">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="D88">
-        <v>4.7</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E88">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="F88" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.4">
@@ -2220,19 +2220,19 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>6.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C89">
-        <v>2.2999999999999998</v>
+        <v>3</v>
       </c>
       <c r="D89">
-        <v>4.4000000000000004</v>
+        <v>1.3</v>
       </c>
       <c r="E89">
-        <v>1.3</v>
+        <v>0.2</v>
       </c>
       <c r="F89" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.4">
@@ -2240,19 +2240,19 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>5.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C90">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="D90">
-        <v>4.0999999999999996</v>
+        <v>1.4</v>
       </c>
       <c r="E90">
-        <v>1.3</v>
+        <v>0.2</v>
       </c>
       <c r="F90" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.4">
@@ -2260,19 +2260,19 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>5.5</v>
+        <v>7.7</v>
       </c>
       <c r="C91">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="D91">
-        <v>4</v>
+        <v>6.9</v>
       </c>
       <c r="E91">
-        <v>1.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F91" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.4">
@@ -2280,16 +2280,16 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="C92">
-        <v>2.6</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D92">
-        <v>4.4000000000000004</v>
+        <v>3.3</v>
       </c>
       <c r="E92">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="s">
         <v>6</v>
@@ -2300,16 +2300,16 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="C93">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="D93">
-        <v>4.5999999999999996</v>
+        <v>3.9</v>
       </c>
       <c r="E93">
-        <v>1.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F93" t="s">
         <v>6</v>
@@ -2320,19 +2320,19 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>5.8</v>
+        <v>6.3</v>
       </c>
       <c r="C94">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="D94">
-        <v>4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E94">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="F94" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.4">
@@ -2340,19 +2340,19 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="C95">
-        <v>2.2999999999999998</v>
+        <v>3</v>
       </c>
       <c r="D95">
-        <v>3.3</v>
+        <v>1.4</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F95" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.4">
@@ -2360,19 +2360,19 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>5.6</v>
+        <v>5</v>
       </c>
       <c r="C96">
-        <v>2.7</v>
+        <v>3.4</v>
       </c>
       <c r="D96">
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="E96">
-        <v>1.3</v>
+        <v>0.2</v>
       </c>
       <c r="F96" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.4">
@@ -2380,19 +2380,19 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>5.7</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C97">
-        <v>3</v>
+        <v>3.8</v>
       </c>
       <c r="D97">
-        <v>4.2</v>
+        <v>1.9</v>
       </c>
       <c r="E97">
-        <v>1.2</v>
+        <v>0.4</v>
       </c>
       <c r="F97" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.4">
@@ -2400,19 +2400,19 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>5.7</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C98">
-        <v>2.9</v>
+        <v>3.8</v>
       </c>
       <c r="D98">
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="E98">
-        <v>1.3</v>
+        <v>0.3</v>
       </c>
       <c r="F98" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.4">
@@ -2420,13 +2420,13 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>6.2</v>
+        <v>6.6</v>
       </c>
       <c r="C99">
         <v>2.9</v>
       </c>
       <c r="D99">
-        <v>4.3</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E99">
         <v>1.3</v>
@@ -2440,16 +2440,16 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>5.0999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="C100">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="D100">
-        <v>3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E100">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="F100" t="s">
         <v>6</v>
@@ -2460,19 +2460,19 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
       <c r="C101">
-        <v>2.8</v>
+        <v>4</v>
       </c>
       <c r="D101">
-        <v>4.0999999999999996</v>
+        <v>1.2</v>
       </c>
       <c r="E101">
-        <v>1.3</v>
+        <v>0.2</v>
       </c>
       <c r="F101" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.4">
@@ -2483,13 +2483,13 @@
         <v>6.3</v>
       </c>
       <c r="C102">
-        <v>3.3</v>
+        <v>2.9</v>
       </c>
       <c r="D102">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="E102">
-        <v>2.5</v>
+        <v>1.8</v>
       </c>
       <c r="F102" t="s">
         <v>7</v>
@@ -2500,19 +2500,19 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="C103">
-        <v>2.7</v>
+        <v>3.7</v>
       </c>
       <c r="D103">
-        <v>5.0999999999999996</v>
+        <v>1.5</v>
       </c>
       <c r="E103">
-        <v>1.9</v>
+        <v>0.2</v>
       </c>
       <c r="F103" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.4">
@@ -2520,16 +2520,16 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>7.1</v>
+        <v>5.8</v>
       </c>
       <c r="C104">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="D104">
-        <v>5.9</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E104">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
       <c r="F104" t="s">
         <v>7</v>
@@ -2540,16 +2540,16 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>6.3</v>
+        <v>6.5</v>
       </c>
       <c r="C105">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="D105">
-        <v>5.6</v>
+        <v>5.2</v>
       </c>
       <c r="E105">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="F105" t="s">
         <v>7</v>
@@ -2560,19 +2560,19 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="C106">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D106">
-        <v>5.8</v>
+        <v>1.6</v>
       </c>
       <c r="E106">
-        <v>2.2000000000000002</v>
+        <v>0.6</v>
       </c>
       <c r="F106" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.4">
@@ -2580,19 +2580,19 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>7.6</v>
+        <v>5.7</v>
       </c>
       <c r="C107">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="D107">
-        <v>6.6</v>
+        <v>4.5</v>
       </c>
       <c r="E107">
-        <v>2.1</v>
+        <v>1.3</v>
       </c>
       <c r="F107" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.4">
@@ -2600,19 +2600,19 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>4.9000000000000004</v>
+        <v>5.9</v>
       </c>
       <c r="C108">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="D108">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E108">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="F108" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.4">
@@ -2620,16 +2620,16 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>7.3</v>
+        <v>6.7</v>
       </c>
       <c r="C109">
-        <v>2.9</v>
+        <v>3.3</v>
       </c>
       <c r="D109">
-        <v>6.3</v>
+        <v>5.7</v>
       </c>
       <c r="E109">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="F109" t="s">
         <v>7</v>
@@ -2640,19 +2640,19 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>6.7</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C110">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="D110">
-        <v>5.8</v>
+        <v>1.4</v>
       </c>
       <c r="E110">
-        <v>1.8</v>
+        <v>0.2</v>
       </c>
       <c r="F110" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.4">
@@ -2660,16 +2660,16 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>7.2</v>
+        <v>7.7</v>
       </c>
       <c r="C111">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="D111">
-        <v>6.1</v>
+        <v>6.7</v>
       </c>
       <c r="E111">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F111" t="s">
         <v>7</v>
@@ -2680,19 +2680,19 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>6.5</v>
+        <v>5.4</v>
       </c>
       <c r="C112">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="D112">
-        <v>5.0999999999999996</v>
+        <v>1.7</v>
       </c>
       <c r="E112">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="F112" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.4">
@@ -2700,16 +2700,16 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>6.4</v>
+        <v>5.6</v>
       </c>
       <c r="C113">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
       <c r="D113">
-        <v>5.3</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E113">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="F113" t="s">
         <v>7</v>
@@ -2720,19 +2720,19 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>6.8</v>
+        <v>6.4</v>
       </c>
       <c r="C114">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="D114">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="E114">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="F114" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.4">
@@ -2740,19 +2740,19 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>5.7</v>
+        <v>5.5</v>
       </c>
       <c r="C115">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="D115">
-        <v>5</v>
+        <v>3.8</v>
       </c>
       <c r="E115">
-        <v>2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F115" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.4">
@@ -2760,16 +2760,16 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>5.8</v>
+        <v>6.5</v>
       </c>
       <c r="C116">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="D116">
         <v>5.0999999999999996</v>
       </c>
       <c r="E116">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="F116" t="s">
         <v>7</v>
@@ -2780,19 +2780,19 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
       <c r="C117">
-        <v>3.2</v>
+        <v>4.2</v>
       </c>
       <c r="D117">
-        <v>5.3</v>
+        <v>1.4</v>
       </c>
       <c r="E117">
-        <v>2.2999999999999998</v>
+        <v>0.2</v>
       </c>
       <c r="F117" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.4">
@@ -2800,19 +2800,19 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>6.5</v>
+        <v>4.7</v>
       </c>
       <c r="C118">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="D118">
-        <v>5.5</v>
+        <v>1.6</v>
       </c>
       <c r="E118">
-        <v>1.8</v>
+        <v>0.2</v>
       </c>
       <c r="F118" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.4">
@@ -2820,19 +2820,19 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>7.7</v>
+        <v>6.1</v>
       </c>
       <c r="C119">
-        <v>3.8</v>
+        <v>3</v>
       </c>
       <c r="D119">
-        <v>6.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E119">
-        <v>2.2000000000000002</v>
+        <v>1.4</v>
       </c>
       <c r="F119" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.4">
@@ -2840,19 +2840,19 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>7.7</v>
+        <v>6</v>
       </c>
       <c r="C120">
-        <v>2.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D120">
-        <v>6.9</v>
+        <v>4</v>
       </c>
       <c r="E120">
-        <v>2.2999999999999998</v>
+        <v>1</v>
       </c>
       <c r="F120" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.4">
@@ -2860,16 +2860,16 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>6</v>
+        <v>6.9</v>
       </c>
       <c r="C121">
-        <v>2.2000000000000002</v>
+        <v>3.1</v>
       </c>
       <c r="D121">
-        <v>5</v>
+        <v>5.4</v>
       </c>
       <c r="E121">
-        <v>1.5</v>
+        <v>2.1</v>
       </c>
       <c r="F121" t="s">
         <v>7</v>
@@ -2880,16 +2880,16 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>6.9</v>
+        <v>7.6</v>
       </c>
       <c r="C122">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="D122">
-        <v>5.7</v>
+        <v>6.6</v>
       </c>
       <c r="E122">
-        <v>2.2999999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="F122" t="s">
         <v>7</v>
@@ -2900,19 +2900,19 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>5.6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C123">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="D123">
-        <v>4.9000000000000004</v>
+        <v>1.4</v>
       </c>
       <c r="E123">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="F123" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.4">
@@ -2920,16 +2920,16 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>7.7</v>
+        <v>6.8</v>
       </c>
       <c r="C124">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="D124">
-        <v>6.7</v>
+        <v>5.5</v>
       </c>
       <c r="E124">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="F124" t="s">
         <v>7</v>
@@ -2943,16 +2943,16 @@
         <v>6.3</v>
       </c>
       <c r="C125">
-        <v>2.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D125">
-        <v>4.9000000000000004</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E125">
-        <v>1.8</v>
+        <v>1.3</v>
       </c>
       <c r="F125" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.4">
@@ -2960,16 +2960,16 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>6.7</v>
+        <v>6.3</v>
       </c>
       <c r="C126">
         <v>3.3</v>
       </c>
       <c r="D126">
-        <v>5.7</v>
+        <v>6</v>
       </c>
       <c r="E126">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="F126" t="s">
         <v>7</v>
@@ -2980,13 +2980,13 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>7.2</v>
+        <v>6.2</v>
       </c>
       <c r="C127">
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
       <c r="D127">
-        <v>6</v>
+        <v>4.8</v>
       </c>
       <c r="E127">
         <v>1.8</v>
@@ -3000,19 +3000,19 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>6.2</v>
+        <v>4.8</v>
       </c>
       <c r="C128">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="D128">
-        <v>4.8</v>
+        <v>1.6</v>
       </c>
       <c r="E128">
-        <v>1.8</v>
+        <v>0.2</v>
       </c>
       <c r="F128" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.4">
@@ -3020,16 +3020,16 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>6.1</v>
+        <v>6.9</v>
       </c>
       <c r="C129">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="D129">
-        <v>4.9000000000000004</v>
+        <v>5.7</v>
       </c>
       <c r="E129">
-        <v>1.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F129" t="s">
         <v>7</v>
@@ -3040,16 +3040,16 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>6.4</v>
+        <v>6.7</v>
       </c>
       <c r="C130">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="D130">
-        <v>5.6</v>
+        <v>5.2</v>
       </c>
       <c r="E130">
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F130" t="s">
         <v>7</v>
@@ -3060,19 +3060,19 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>7.2</v>
+        <v>5.6</v>
       </c>
       <c r="C131">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="D131">
-        <v>5.8</v>
+        <v>4.2</v>
       </c>
       <c r="E131">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="F131" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.4">
@@ -3080,19 +3080,19 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>7.4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C132">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="D132">
-        <v>6.1</v>
+        <v>1.5</v>
       </c>
       <c r="E132">
-        <v>1.9</v>
+        <v>0.2</v>
       </c>
       <c r="F132" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.4">
@@ -3100,19 +3100,19 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C133">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
       <c r="D133">
-        <v>6.4</v>
+        <v>1.3</v>
       </c>
       <c r="E133">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="F133" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.4">
@@ -3120,19 +3120,19 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>6.4</v>
+        <v>6.2</v>
       </c>
       <c r="C134">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="D134">
-        <v>5.6</v>
+        <v>4.3</v>
       </c>
       <c r="E134">
-        <v>2.2000000000000002</v>
+        <v>1.3</v>
       </c>
       <c r="F134" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.4">
@@ -3140,19 +3140,19 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>6.3</v>
+        <v>6</v>
       </c>
       <c r="C135">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="D135">
         <v>5.0999999999999996</v>
       </c>
       <c r="E135">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="F135" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.4">
@@ -3160,19 +3160,19 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>6.1</v>
+        <v>5.7</v>
       </c>
       <c r="C136">
         <v>2.6</v>
       </c>
       <c r="D136">
-        <v>5.6</v>
+        <v>3.5</v>
       </c>
       <c r="E136">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="F136" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.4">
@@ -3180,19 +3180,19 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>7.7</v>
+        <v>6.3</v>
       </c>
       <c r="C137">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="D137">
-        <v>6.1</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E137">
-        <v>2.2999999999999998</v>
+        <v>1.5</v>
       </c>
       <c r="F137" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.4">
@@ -3200,19 +3200,19 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>6.3</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C138">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="D138">
-        <v>5.6</v>
+        <v>1</v>
       </c>
       <c r="E138">
-        <v>2.4</v>
+        <v>0.2</v>
       </c>
       <c r="F138" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.4">
@@ -3220,19 +3220,19 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>6.4</v>
+        <v>6.5</v>
       </c>
       <c r="C139">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="D139">
-        <v>5.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E139">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="F139" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.4">
@@ -3240,19 +3240,19 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C140">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D140">
-        <v>4.8</v>
+        <v>1.3</v>
       </c>
       <c r="E140">
-        <v>1.8</v>
+        <v>0.3</v>
       </c>
       <c r="F140" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.4">
@@ -3260,16 +3260,16 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>6.9</v>
+        <v>6</v>
       </c>
       <c r="C141">
-        <v>3.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D141">
-        <v>5.4</v>
+        <v>5</v>
       </c>
       <c r="E141">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="F141" t="s">
         <v>7</v>
@@ -3280,19 +3280,19 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>6.7</v>
+        <v>6.1</v>
       </c>
       <c r="C142">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="D142">
-        <v>5.6</v>
+        <v>4.7</v>
       </c>
       <c r="E142">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="F142" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.4">
@@ -3300,19 +3300,19 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>6.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C143">
         <v>3.1</v>
       </c>
       <c r="D143">
-        <v>5.0999999999999996</v>
+        <v>1.5</v>
       </c>
       <c r="E143">
-        <v>2.2999999999999998</v>
+        <v>0.2</v>
       </c>
       <c r="F143" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.4">
@@ -3320,16 +3320,16 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>5.8</v>
+        <v>6.4</v>
       </c>
       <c r="C144">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="D144">
-        <v>5.0999999999999996</v>
+        <v>5.5</v>
       </c>
       <c r="E144">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="F144" t="s">
         <v>7</v>
@@ -3340,19 +3340,19 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>6.8</v>
+        <v>6.7</v>
       </c>
       <c r="C145">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="D145">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E145">
-        <v>2.2999999999999998</v>
+        <v>1.4</v>
       </c>
       <c r="F145" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.4">
@@ -3363,13 +3363,13 @@
         <v>6.7</v>
       </c>
       <c r="C146">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="D146">
-        <v>5.7</v>
+        <v>5.6</v>
       </c>
       <c r="E146">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="F146" t="s">
         <v>7</v>
@@ -3380,13 +3380,13 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>6.7</v>
+        <v>7.7</v>
       </c>
       <c r="C147">
         <v>3</v>
       </c>
       <c r="D147">
-        <v>5.2</v>
+        <v>6.1</v>
       </c>
       <c r="E147">
         <v>2.2999999999999998</v>
@@ -3400,19 +3400,19 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>6.3</v>
+        <v>5.2</v>
       </c>
       <c r="C148">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="D148">
-        <v>5</v>
+        <v>3.9</v>
       </c>
       <c r="E148">
-        <v>1.9</v>
+        <v>1.4</v>
       </c>
       <c r="F148" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.4">
@@ -3420,13 +3420,13 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>6.5</v>
+        <v>7.7</v>
       </c>
       <c r="C149">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="D149">
-        <v>5.2</v>
+        <v>6.7</v>
       </c>
       <c r="E149">
         <v>2</v>
@@ -3440,19 +3440,19 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>6.2</v>
+        <v>5</v>
       </c>
       <c r="C150">
         <v>3.4</v>
       </c>
       <c r="D150">
-        <v>5.4</v>
+        <v>1.6</v>
       </c>
       <c r="E150">
-        <v>2.2999999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="F150" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.4">
@@ -3460,16 +3460,16 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>5.9</v>
+        <v>6.3</v>
       </c>
       <c r="C151">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="D151">
-        <v>5.0999999999999996</v>
+        <v>5</v>
       </c>
       <c r="E151">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="F151" t="s">
         <v>7</v>
@@ -3478,5 +3478,6 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>